<commit_message>
final-duca se pe apa sambetei sa nu te mai vad scarba
</commit_message>
<xml_diff>
--- a/Licenta/wwwroot/UploadAccomodationRequests/AccomodationRequests.xlsx
+++ b/Licenta/wwwroot/UploadAccomodationRequests/AccomodationRequests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -136,6 +136,9 @@
   <si>
     <t>e</t>
   </si>
+  <si>
+    <t>CNP Student</t>
+  </si>
 </sst>
 </file>
 
@@ -170,8 +173,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R81"/>
+  <dimension ref="A1:S82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D72" workbookViewId="0">
-      <selection activeCell="J81" sqref="J81"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="R81" sqref="R81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,9 +468,10 @@
     <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,8 +514,11 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -565,8 +573,11 @@
       <c r="R2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S2" s="1">
+        <v>1866498460482</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -621,8 +632,11 @@
       <c r="R3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S3" s="1">
+        <v>1956450348934</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -677,8 +691,11 @@
       <c r="R4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S4" s="1">
+        <v>1308263284153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -733,8 +750,11 @@
       <c r="R5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S5" s="1">
+        <v>2617062211854</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -789,8 +809,11 @@
       <c r="R6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6" s="1">
+        <v>2838845331313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -845,8 +868,11 @@
       <c r="R7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S7" s="1">
+        <v>1867466742476</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -901,8 +927,11 @@
       <c r="R8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S8" s="1">
+        <v>1551931197765</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -957,8 +986,11 @@
       <c r="R9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S9" s="1">
+        <v>1028418149256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1013,8 +1045,11 @@
       <c r="R10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S10" s="1">
+        <v>1844715644239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1069,8 +1104,11 @@
       <c r="R11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11" s="1">
+        <v>1726468814747</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1125,8 +1163,11 @@
       <c r="R12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S12" s="1">
+        <v>1970877973536</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1181,8 +1222,11 @@
       <c r="R13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S13" s="1">
+        <v>2395660506685</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1237,8 +1281,11 @@
       <c r="R14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S14" s="1">
+        <v>1077379103562</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1293,8 +1340,11 @@
       <c r="R15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S15" s="1">
+        <v>2630780501605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1349,8 +1399,11 @@
       <c r="R16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S16" s="1">
+        <v>2242843027580</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1405,8 +1458,11 @@
       <c r="R17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S17" s="1">
+        <v>2584219018245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1461,8 +1517,11 @@
       <c r="R18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S18" s="1">
+        <v>2818583192592</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1517,8 +1576,11 @@
       <c r="R19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S19" s="1">
+        <v>1239160950618</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1573,8 +1635,11 @@
       <c r="R20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S20" s="1">
+        <v>2797469824415</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1629,8 +1694,11 @@
       <c r="R21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S21" s="1">
+        <v>2402082685256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1685,8 +1753,11 @@
       <c r="R22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S22" s="1">
+        <v>2688987461653</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1741,8 +1812,11 @@
       <c r="R23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S23" s="1">
+        <v>1831122074537</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1797,8 +1871,11 @@
       <c r="R24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S24" s="1">
+        <v>1622857464513</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1853,8 +1930,11 @@
       <c r="R25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S25" s="1">
+        <v>1410551152313</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1909,8 +1989,11 @@
       <c r="R26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S26" s="1">
+        <v>2827660921748</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1965,8 +2048,11 @@
       <c r="R27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S27" s="1">
+        <v>2390727251253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2021,8 +2107,11 @@
       <c r="R28" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S28" s="1">
+        <v>1172233458805</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2077,8 +2166,11 @@
       <c r="R29" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S29" s="1">
+        <v>2917067566297</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2133,8 +2225,11 @@
       <c r="R30" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S30" s="1">
+        <v>2609388339425</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2189,8 +2284,11 @@
       <c r="R31" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S31" s="1">
+        <v>1964559432191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2245,8 +2343,11 @@
       <c r="R32" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S32" s="1">
+        <v>1946278818054</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2301,8 +2402,11 @@
       <c r="R33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S33" s="1">
+        <v>2292262889763</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2357,8 +2461,11 @@
       <c r="R34" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S34" s="1">
+        <v>2201634315915</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2413,8 +2520,11 @@
       <c r="R35" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S35" s="1">
+        <v>2131541966656</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2469,8 +2579,11 @@
       <c r="R36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S36" s="1">
+        <v>2782358271726</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2525,8 +2638,11 @@
       <c r="R37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S37" s="1">
+        <v>1220663273992</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2581,8 +2697,11 @@
       <c r="R38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S38" s="1">
+        <v>1187943554245</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2637,8 +2756,11 @@
       <c r="R39" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S39" s="1">
+        <v>2764498400490</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2693,8 +2815,11 @@
       <c r="R40" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S40" s="1">
+        <v>2947341887451</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2749,8 +2874,11 @@
       <c r="R41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S41" s="1">
+        <v>1792235514769</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2805,8 +2933,11 @@
       <c r="R42" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S42" s="1">
+        <v>1141884945479</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2861,8 +2992,11 @@
       <c r="R43" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S43" s="1">
+        <v>2563032073092</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2917,8 +3051,11 @@
       <c r="R44" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S44" s="1">
+        <v>2869301852376</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2973,8 +3110,11 @@
       <c r="R45" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S45" s="1">
+        <v>1744363137926</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3029,8 +3169,11 @@
       <c r="R46" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S46" s="1">
+        <v>1280816175939</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3085,8 +3228,11 @@
       <c r="R47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S47" s="1">
+        <v>2952734379822</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3141,8 +3287,11 @@
       <c r="R48" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S48" s="1">
+        <v>2973916444172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3197,8 +3346,11 @@
       <c r="R49" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S49" s="1">
+        <v>1430381274793</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3253,8 +3405,11 @@
       <c r="R50" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S50" s="1">
+        <v>1327216977921</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3309,8 +3464,11 @@
       <c r="R51" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S51" s="1">
+        <v>2788406798196</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3365,8 +3523,11 @@
       <c r="R52" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S52" s="1">
+        <v>1319441022279</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3421,8 +3582,11 @@
       <c r="R53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S53" s="1">
+        <v>1551099514261</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3477,8 +3641,11 @@
       <c r="R54" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S54" s="1">
+        <v>1347096980955</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3533,8 +3700,11 @@
       <c r="R55" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S55" s="1">
+        <v>1357712550842</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3589,8 +3759,11 @@
       <c r="R56" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S56" s="1">
+        <v>2051268234049</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3645,8 +3818,11 @@
       <c r="R57" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S57" s="1">
+        <v>2998558867457</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3701,8 +3877,11 @@
       <c r="R58" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S58" s="1">
+        <v>1750863814702</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3725,7 +3904,7 @@
         <v>5</v>
       </c>
       <c r="H59">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I59" t="s">
         <v>36</v>
@@ -3757,8 +3936,11 @@
       <c r="R59" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S59" s="1">
+        <v>2763023401601</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3813,8 +3995,11 @@
       <c r="R60" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S60" s="1">
+        <v>2923416059733</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3869,8 +4054,11 @@
       <c r="R61" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S61" s="1">
+        <v>1778600630388</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3925,8 +4113,11 @@
       <c r="R62" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S62" s="1">
+        <v>1761002685109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3981,8 +4172,11 @@
       <c r="R63" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S63" s="1">
+        <v>1947114548534</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4037,8 +4231,11 @@
       <c r="R64" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S64" s="1">
+        <v>1325104150600</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4093,8 +4290,11 @@
       <c r="R65" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S65" s="1">
+        <v>1033536046282</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4149,8 +4349,11 @@
       <c r="R66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S66" s="1">
+        <v>1538454843096</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4205,8 +4408,11 @@
       <c r="R67" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S67" s="1">
+        <v>2517329660578</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4261,8 +4467,11 @@
       <c r="R68" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S68" s="1">
+        <v>2085387466684</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4317,8 +4526,11 @@
       <c r="R69" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S69" s="1">
+        <v>1043096233960</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4373,8 +4585,11 @@
       <c r="R70" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S70" s="1">
+        <v>1817301513165</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4429,8 +4644,11 @@
       <c r="R71" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S71" s="1">
+        <v>1127377173910</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4485,8 +4703,11 @@
       <c r="R72" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S72" s="1">
+        <v>1881901990703</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4541,8 +4762,11 @@
       <c r="R73" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S73" s="1">
+        <v>2189581479668</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4597,8 +4821,11 @@
       <c r="R74" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S74" s="1">
+        <v>1780783783387</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4653,8 +4880,11 @@
       <c r="R75" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S75" s="1">
+        <v>2672573544366</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4709,8 +4939,11 @@
       <c r="R76" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S76" s="1">
+        <v>2939386868430</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4765,8 +4998,11 @@
       <c r="R77" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S77" s="1">
+        <v>2144097372935</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4821,8 +5057,11 @@
       <c r="R78" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S78" s="1">
+        <v>1534771783436</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4877,8 +5116,11 @@
       <c r="R79" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S79" s="1">
+        <v>1182655611322</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4933,8 +5175,11 @@
       <c r="R80" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S80" s="1">
+        <v>1892127160034</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4942,10 +5187,10 @@
         <v>13</v>
       </c>
       <c r="C81" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D81" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="E81" t="s">
         <v>36</v>
@@ -4956,11 +5201,11 @@
       <c r="G81">
         <v>1</v>
       </c>
-      <c r="H81">
-        <v>2</v>
-      </c>
-      <c r="I81">
-        <v>3</v>
+      <c r="H81" t="s">
+        <v>36</v>
+      </c>
+      <c r="I81" t="s">
+        <v>36</v>
       </c>
       <c r="J81" t="s">
         <v>36</v>
@@ -4987,8 +5232,14 @@
         <v>36</v>
       </c>
       <c r="R81">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="S81" s="1">
+        <v>2123456789123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S82" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>